<commit_message>
Updating clustered column trials and Power BI dashboard
</commit_message>
<xml_diff>
--- a/ExcelCalcs/ClusterColumnChartTest.xlsx
+++ b/ExcelCalcs/ClusterColumnChartTest.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d84190290dfea8be/Documents/CodeInstitute/vscode-projects/Capstone_Evaluating_Domestic_Electrification_Measures/ExcelCalcs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="11_AD4DB114E441178AC67DF43B0E56FED6683EDF26" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50D3DEFD-D351-430C-A008-4E26CCEFC9A5}"/>
+  <xr:revisionPtr revIDLastSave="178" documentId="11_AD4DB114E441178AC67DF43B0E56FED6683EDF26" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97F3F0E1-0DFE-4824-86EC-5FD03EAB97BC}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="7500_60" sheetId="1" r:id="rId1"/>
+    <sheet name="Test" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,21 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
-  <si>
-    <t>Car replacement if applicable</t>
-  </si>
-  <si>
-    <t>Loan interest if applicable</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="13">
   <si>
     <t>Fuel</t>
   </si>
   <si>
     <t>Maintenance</t>
-  </si>
-  <si>
-    <t>Total Tonnes CO2 emissions</t>
   </si>
   <si>
     <t>Petrol</t>
@@ -71,7 +62,19 @@
     <t>Use_Range_mi</t>
   </si>
   <si>
-    <t>Car Price + any charger (Tot capital repayments if loan).</t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Car Price + charger</t>
+  </si>
+  <si>
+    <t>Car replacement</t>
+  </si>
+  <si>
+    <t>Loan interest</t>
+  </si>
+  <si>
+    <t>CO2 emissions Tonnes</t>
   </si>
 </sst>
 </file>
@@ -143,6 +146,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -408,45 +415,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="11.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="116" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -460,7 +469,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E2" s="2">
         <v>13901</v>
@@ -492,7 +501,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E3" s="2">
         <v>10321</v>
@@ -521,28 +530,28 @@
         <v>60</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>11219</v>
+        <v>0</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="2">
-        <v>2179.5155183796978</v>
+        <v>0</v>
       </c>
       <c r="H4" s="2">
-        <v>1150.6486340000001</v>
+        <v>0</v>
       </c>
       <c r="I4" s="2">
-        <v>4156</v>
+        <v>0</v>
       </c>
       <c r="J4" s="3">
-        <v>1.8124705962000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -559,22 +568,22 @@
         <v>5</v>
       </c>
       <c r="E5" s="2">
-        <v>8176</v>
+        <v>11219</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
       </c>
       <c r="G5" s="2">
-        <v>1588.3518030370274</v>
+        <v>2179.5155183796978</v>
       </c>
       <c r="H5" s="2">
-        <v>3704.64</v>
+        <v>1150.6486340000001</v>
       </c>
       <c r="I5" s="2">
-        <v>5988</v>
+        <v>4156</v>
       </c>
       <c r="J5" s="3">
-        <v>6.3741599999999998</v>
+        <v>1.8124705962000001</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -585,28 +594,28 @@
         <v>60</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E6" s="2">
-        <v>11221</v>
+        <v>8176</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
       </c>
       <c r="G6" s="2">
-        <v>2179.9040584489339</v>
+        <v>1588.3518030370274</v>
       </c>
       <c r="H6" s="2">
-        <v>1083.5649108</v>
+        <v>3704.64</v>
       </c>
       <c r="I6" s="2">
-        <v>4156</v>
+        <v>5988</v>
       </c>
       <c r="J6" s="3">
-        <v>1.7068021304400001</v>
+        <v>6.3741599999999998</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -617,28 +626,28 @@
         <v>60</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>8177</v>
+        <v>0</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="2">
-        <v>1588.5460730716454</v>
+        <v>0</v>
       </c>
       <c r="H7" s="2">
-        <v>3704.64</v>
+        <v>0</v>
       </c>
       <c r="I7" s="2">
-        <v>5988</v>
+        <v>0</v>
       </c>
       <c r="J7" s="3">
-        <v>6.3741599999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -649,28 +658,28 @@
         <v>60</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E8" s="2">
-        <v>14619</v>
+        <v>11221</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
       </c>
       <c r="G8" s="2">
-        <v>2840.0336360810056</v>
+        <v>2179.9040584489339</v>
       </c>
       <c r="H8" s="2">
-        <v>1152.0068779999999</v>
+        <v>1083.5649108</v>
       </c>
       <c r="I8" s="2">
         <v>4156</v>
       </c>
       <c r="J8" s="3">
-        <v>1.8146100654000001</v>
+        <v>1.7068021304400001</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -681,19 +690,19 @@
         <v>60</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E9" s="2">
-        <v>10895</v>
+        <v>8177</v>
       </c>
       <c r="F9" s="2">
         <v>0</v>
       </c>
       <c r="G9" s="2">
-        <v>2116.5720271634555</v>
+        <v>1588.5460730716454</v>
       </c>
       <c r="H9" s="2">
         <v>3704.64</v>
@@ -713,28 +722,28 @@
         <v>60</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="2">
-        <v>16092</v>
+        <v>0</v>
       </c>
       <c r="F10" s="2">
         <v>0</v>
       </c>
       <c r="G10" s="2">
-        <v>3126.1933970733662</v>
+        <v>0</v>
       </c>
       <c r="H10" s="2">
-        <v>1178.0862036000001</v>
+        <v>0</v>
       </c>
       <c r="I10" s="2">
-        <v>4156</v>
+        <v>0</v>
       </c>
       <c r="J10" s="3">
-        <v>1.8556895134800002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -745,28 +754,28 @@
         <v>60</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="2">
-        <v>12073</v>
+        <v>14619</v>
       </c>
       <c r="F11" s="2">
         <v>0</v>
       </c>
       <c r="G11" s="2">
-        <v>2345.4221279434969</v>
+        <v>2840.0336360810056</v>
       </c>
       <c r="H11" s="2">
-        <v>3704.64</v>
+        <v>1152.0068779999999</v>
       </c>
       <c r="I11" s="2">
-        <v>5988</v>
+        <v>4156</v>
       </c>
       <c r="J11" s="3">
-        <v>6.3741599999999998</v>
+        <v>1.8146100654000001</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -777,28 +786,28 @@
         <v>60</v>
       </c>
       <c r="C12">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E12" s="2">
-        <v>18581</v>
+        <v>10895</v>
       </c>
       <c r="F12" s="2">
         <v>0</v>
       </c>
       <c r="G12" s="2">
-        <v>3609.7315132376475</v>
+        <v>2116.5720271634555</v>
       </c>
       <c r="H12" s="2">
-        <v>1173.1288732</v>
+        <v>3704.64</v>
       </c>
       <c r="I12" s="2">
-        <v>4156</v>
+        <v>5988</v>
       </c>
       <c r="J12" s="3">
-        <v>1.8478808607599999</v>
+        <v>6.3741599999999998</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -809,28 +818,28 @@
         <v>60</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E13" s="2">
-        <v>14065</v>
+        <v>0</v>
       </c>
       <c r="F13" s="2">
         <v>0</v>
       </c>
       <c r="G13" s="2">
-        <v>2732.408036902616</v>
+        <v>0</v>
       </c>
       <c r="H13" s="2">
-        <v>3704.64</v>
+        <v>0</v>
       </c>
       <c r="I13" s="2">
-        <v>5988</v>
+        <v>0</v>
       </c>
       <c r="J13" s="3">
-        <v>6.3741599999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -841,28 +850,28 @@
         <v>60</v>
       </c>
       <c r="C14">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E14" s="2">
-        <v>22881</v>
+        <v>16092</v>
       </c>
       <c r="F14" s="2">
         <v>0</v>
       </c>
       <c r="G14" s="2">
-        <v>4445.0926620951841</v>
+        <v>3126.1933970733662</v>
       </c>
       <c r="H14" s="2">
-        <v>1206.4917172</v>
+        <v>1178.0862036000001</v>
       </c>
       <c r="I14" s="2">
         <v>4156</v>
       </c>
       <c r="J14" s="3">
-        <v>1.90043310996</v>
+        <v>1.8556895134800002</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -873,19 +882,19 @@
         <v>60</v>
       </c>
       <c r="C15">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E15" s="2">
-        <v>17505</v>
+        <v>12073</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
       </c>
       <c r="G15" s="2">
-        <v>3400.6969559886452</v>
+        <v>2345.4221279434969</v>
       </c>
       <c r="H15" s="2">
         <v>3704.64</v>
@@ -905,28 +914,28 @@
         <v>60</v>
       </c>
       <c r="C16">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D16" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="2">
-        <v>26124</v>
+        <v>0</v>
       </c>
       <c r="F16" s="2">
         <v>0</v>
       </c>
       <c r="G16" s="2">
-        <v>5075.110384361461</v>
+        <v>0</v>
       </c>
       <c r="H16" s="2">
-        <v>1211.7352676</v>
+        <v>0</v>
       </c>
       <c r="I16" s="2">
-        <v>4156</v>
+        <v>0</v>
       </c>
       <c r="J16" s="3">
-        <v>1.9086926086800002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -937,28 +946,28 @@
         <v>60</v>
       </c>
       <c r="C17">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
       </c>
       <c r="E17" s="2">
-        <v>20099</v>
+        <v>18581</v>
       </c>
       <c r="F17" s="2">
         <v>0</v>
       </c>
       <c r="G17" s="2">
-        <v>3904.6334257878193</v>
+        <v>3609.7315132376475</v>
       </c>
       <c r="H17" s="2">
-        <v>3704.64</v>
+        <v>1173.1288732</v>
       </c>
       <c r="I17" s="2">
-        <v>5988</v>
+        <v>4156</v>
       </c>
       <c r="J17" s="3">
-        <v>6.3741599999999998</v>
+        <v>1.8478808607599999</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -969,28 +978,28 @@
         <v>60</v>
       </c>
       <c r="C18">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E18" s="2">
-        <v>27151</v>
+        <v>14065</v>
       </c>
       <c r="F18" s="2">
         <v>0</v>
       </c>
       <c r="G18" s="2">
-        <v>5274.6257099141794</v>
+        <v>2732.408036902616</v>
       </c>
       <c r="H18" s="2">
-        <v>1221.2138332</v>
+        <v>3704.64</v>
       </c>
       <c r="I18" s="2">
-        <v>4156</v>
+        <v>5988</v>
       </c>
       <c r="J18" s="3">
-        <v>1.92362298876</v>
+        <v>6.3741599999999998</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
@@ -1001,28 +1010,1180 @@
         <v>60</v>
       </c>
       <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>7500</v>
+      </c>
+      <c r="B20">
+        <v>60</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="2">
+        <v>22881</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
+        <v>4445.0926620951841</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1206.4917172</v>
+      </c>
+      <c r="I20" s="2">
+        <v>4156</v>
+      </c>
+      <c r="J20" s="3">
+        <v>1.90043310996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>7500</v>
+      </c>
+      <c r="B21">
+        <v>60</v>
+      </c>
+      <c r="C21">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="2">
+        <v>17505</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2">
+        <v>3400.6969559886452</v>
+      </c>
+      <c r="H21" s="2">
+        <v>3704.64</v>
+      </c>
+      <c r="I21" s="2">
+        <v>5988</v>
+      </c>
+      <c r="J21" s="3">
+        <v>6.3741599999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>7500</v>
+      </c>
+      <c r="B22">
+        <v>60</v>
+      </c>
+      <c r="C22">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>7500</v>
+      </c>
+      <c r="B23">
+        <v>60</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="2">
+        <v>26124</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2">
+        <v>5075.110384361461</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1211.7352676</v>
+      </c>
+      <c r="I23" s="2">
+        <v>4156</v>
+      </c>
+      <c r="J23" s="3">
+        <v>1.9086926086800002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>7500</v>
+      </c>
+      <c r="B24">
+        <v>60</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="2">
+        <v>20099</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0</v>
+      </c>
+      <c r="G24" s="2">
+        <v>3904.6334257878193</v>
+      </c>
+      <c r="H24" s="2">
+        <v>3704.64</v>
+      </c>
+      <c r="I24" s="2">
+        <v>5988</v>
+      </c>
+      <c r="J24" s="3">
+        <v>6.3741599999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>7500</v>
+      </c>
+      <c r="B25">
+        <v>60</v>
+      </c>
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0</v>
+      </c>
+      <c r="J25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>7500</v>
+      </c>
+      <c r="B26">
+        <v>60</v>
+      </c>
+      <c r="C26">
         <v>9</v>
       </c>
-      <c r="D19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="2">
+      <c r="D26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="2">
+        <v>27151</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
+        <v>5274.6257099141794</v>
+      </c>
+      <c r="H26" s="2">
+        <v>1221.2138332</v>
+      </c>
+      <c r="I26" s="2">
+        <v>4156</v>
+      </c>
+      <c r="J26" s="3">
+        <v>1.92362298876</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>7500</v>
+      </c>
+      <c r="B27">
+        <v>60</v>
+      </c>
+      <c r="C27">
+        <v>9</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="2">
         <v>20920</v>
       </c>
-      <c r="F19" s="2">
-        <v>0</v>
-      </c>
-      <c r="G19" s="2">
+      <c r="F27" s="2">
+        <v>0</v>
+      </c>
+      <c r="G27" s="2">
         <v>4064.1291242092234</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H27" s="2">
         <v>3704.64</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I27" s="2">
         <v>5988</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J27" s="3">
         <v>6.3741599999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>7500</v>
+      </c>
+      <c r="B28">
+        <v>60</v>
+      </c>
+      <c r="C28">
+        <v>9</v>
+      </c>
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0</v>
+      </c>
+      <c r="I28" s="2">
+        <v>0</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>7500</v>
+      </c>
+      <c r="B29">
+        <v>75</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0</v>
+      </c>
+      <c r="J29" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>7500</v>
+      </c>
+      <c r="B30">
+        <v>75</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0</v>
+      </c>
+      <c r="I30" s="2">
+        <v>0</v>
+      </c>
+      <c r="J30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>7500</v>
+      </c>
+      <c r="B31">
+        <v>75</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2">
+        <v>0</v>
+      </c>
+      <c r="J31" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>7500</v>
+      </c>
+      <c r="B32">
+        <v>75</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="2">
+        <v>11219</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0</v>
+      </c>
+      <c r="G32" s="2">
+        <v>2179.5155183796978</v>
+      </c>
+      <c r="H32" s="2">
+        <v>1150.6486340000001</v>
+      </c>
+      <c r="I32" s="2">
+        <v>4156</v>
+      </c>
+      <c r="J32" s="3">
+        <v>1.8124705962000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>7500</v>
+      </c>
+      <c r="B33">
+        <v>75</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="2">
+        <v>8176</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0</v>
+      </c>
+      <c r="G33" s="2">
+        <v>1588.3518030370274</v>
+      </c>
+      <c r="H33" s="2">
+        <v>3704.64</v>
+      </c>
+      <c r="I33" s="2">
+        <v>5988</v>
+      </c>
+      <c r="J33" s="3">
+        <v>6.3741599999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>7500</v>
+      </c>
+      <c r="B34">
+        <v>75</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0</v>
+      </c>
+      <c r="I34" s="2">
+        <v>0</v>
+      </c>
+      <c r="J34" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>7500</v>
+      </c>
+      <c r="B35">
+        <v>75</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="2">
+        <v>11221</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0</v>
+      </c>
+      <c r="G35" s="2">
+        <v>2179.9040584489339</v>
+      </c>
+      <c r="H35" s="2">
+        <v>1083.5649108</v>
+      </c>
+      <c r="I35" s="2">
+        <v>4156</v>
+      </c>
+      <c r="J35" s="3">
+        <v>1.7068021304400001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>7500</v>
+      </c>
+      <c r="B36">
+        <v>75</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" s="2">
+        <v>8177</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0</v>
+      </c>
+      <c r="G36" s="2">
+        <v>1588.5460730716454</v>
+      </c>
+      <c r="H36" s="2">
+        <v>3704.64</v>
+      </c>
+      <c r="I36" s="2">
+        <v>5988</v>
+      </c>
+      <c r="J36" s="3">
+        <v>6.3741599999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>7500</v>
+      </c>
+      <c r="B37">
+        <v>75</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0</v>
+      </c>
+      <c r="H37" s="2">
+        <v>0</v>
+      </c>
+      <c r="I37" s="2">
+        <v>0</v>
+      </c>
+      <c r="J37" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>7500</v>
+      </c>
+      <c r="B38">
+        <v>75</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="2">
+        <v>14619</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0</v>
+      </c>
+      <c r="G38" s="2">
+        <v>2840.0336360810056</v>
+      </c>
+      <c r="H38" s="2">
+        <v>1152.0068779999999</v>
+      </c>
+      <c r="I38" s="2">
+        <v>4156</v>
+      </c>
+      <c r="J38" s="3">
+        <v>1.8146100654000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>7500</v>
+      </c>
+      <c r="B39">
+        <v>75</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" s="2">
+        <v>10895</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0</v>
+      </c>
+      <c r="G39" s="2">
+        <v>2116.5720271634555</v>
+      </c>
+      <c r="H39" s="2">
+        <v>3704.64</v>
+      </c>
+      <c r="I39" s="2">
+        <v>5988</v>
+      </c>
+      <c r="J39" s="3">
+        <v>6.3741599999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>7500</v>
+      </c>
+      <c r="B40">
+        <v>75</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="2">
+        <v>0</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0</v>
+      </c>
+      <c r="G40" s="2">
+        <v>0</v>
+      </c>
+      <c r="H40" s="2">
+        <v>0</v>
+      </c>
+      <c r="I40" s="2">
+        <v>0</v>
+      </c>
+      <c r="J40" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>7500</v>
+      </c>
+      <c r="B41">
+        <v>75</v>
+      </c>
+      <c r="C41">
+        <v>5</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="2">
+        <v>16092</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0</v>
+      </c>
+      <c r="G41" s="2">
+        <v>3126.1933970733662</v>
+      </c>
+      <c r="H41" s="2">
+        <v>1178.0862036000001</v>
+      </c>
+      <c r="I41" s="2">
+        <v>4156</v>
+      </c>
+      <c r="J41" s="3">
+        <v>1.8556895134800002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>7500</v>
+      </c>
+      <c r="B42">
+        <v>75</v>
+      </c>
+      <c r="C42">
+        <v>5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42" s="2">
+        <v>12073</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0</v>
+      </c>
+      <c r="G42" s="2">
+        <v>2345.4221279434969</v>
+      </c>
+      <c r="H42" s="2">
+        <v>3704.64</v>
+      </c>
+      <c r="I42" s="2">
+        <v>5988</v>
+      </c>
+      <c r="J42" s="3">
+        <v>6.3741599999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>7500</v>
+      </c>
+      <c r="B43">
+        <v>75</v>
+      </c>
+      <c r="C43">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="2">
+        <v>0</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0</v>
+      </c>
+      <c r="G43" s="2">
+        <v>0</v>
+      </c>
+      <c r="H43" s="2">
+        <v>0</v>
+      </c>
+      <c r="I43" s="2">
+        <v>0</v>
+      </c>
+      <c r="J43" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>7500</v>
+      </c>
+      <c r="B44">
+        <v>75</v>
+      </c>
+      <c r="C44">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" s="2">
+        <v>18581</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0</v>
+      </c>
+      <c r="G44" s="2">
+        <v>3609.7315132376475</v>
+      </c>
+      <c r="H44" s="2">
+        <v>1173.1288732</v>
+      </c>
+      <c r="I44" s="2">
+        <v>4156</v>
+      </c>
+      <c r="J44" s="3">
+        <v>1.8478808607599999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>7500</v>
+      </c>
+      <c r="B45">
+        <v>75</v>
+      </c>
+      <c r="C45">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" s="2">
+        <v>14065</v>
+      </c>
+      <c r="F45" s="2">
+        <v>0</v>
+      </c>
+      <c r="G45" s="2">
+        <v>2732.408036902616</v>
+      </c>
+      <c r="H45" s="2">
+        <v>3704.64</v>
+      </c>
+      <c r="I45" s="2">
+        <v>5988</v>
+      </c>
+      <c r="J45" s="3">
+        <v>6.3741599999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>7500</v>
+      </c>
+      <c r="B46">
+        <v>75</v>
+      </c>
+      <c r="C46">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="2">
+        <v>0</v>
+      </c>
+      <c r="F46" s="2">
+        <v>0</v>
+      </c>
+      <c r="G46" s="2">
+        <v>0</v>
+      </c>
+      <c r="H46" s="2">
+        <v>0</v>
+      </c>
+      <c r="I46" s="2">
+        <v>0</v>
+      </c>
+      <c r="J46" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>7500</v>
+      </c>
+      <c r="B47">
+        <v>75</v>
+      </c>
+      <c r="C47">
+        <v>7</v>
+      </c>
+      <c r="D47" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47" s="2">
+        <v>22881</v>
+      </c>
+      <c r="F47" s="2">
+        <v>0</v>
+      </c>
+      <c r="G47" s="2">
+        <v>4445.0926620951841</v>
+      </c>
+      <c r="H47" s="2">
+        <v>1206.4917172</v>
+      </c>
+      <c r="I47" s="2">
+        <v>4156</v>
+      </c>
+      <c r="J47" s="3">
+        <v>1.90043310996</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>7500</v>
+      </c>
+      <c r="B48">
+        <v>75</v>
+      </c>
+      <c r="C48">
+        <v>7</v>
+      </c>
+      <c r="D48" t="s">
+        <v>2</v>
+      </c>
+      <c r="E48" s="2">
+        <v>17505</v>
+      </c>
+      <c r="F48" s="2">
+        <v>0</v>
+      </c>
+      <c r="G48" s="2">
+        <v>3400.6969559886452</v>
+      </c>
+      <c r="H48" s="2">
+        <v>3704.64</v>
+      </c>
+      <c r="I48" s="2">
+        <v>5988</v>
+      </c>
+      <c r="J48" s="3">
+        <v>6.3741599999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>7500</v>
+      </c>
+      <c r="B49">
+        <v>75</v>
+      </c>
+      <c r="C49">
+        <v>7</v>
+      </c>
+      <c r="D49" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="2">
+        <v>0</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0</v>
+      </c>
+      <c r="G49" s="2">
+        <v>0</v>
+      </c>
+      <c r="H49" s="2">
+        <v>0</v>
+      </c>
+      <c r="I49" s="2">
+        <v>0</v>
+      </c>
+      <c r="J49" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>7500</v>
+      </c>
+      <c r="B50">
+        <v>75</v>
+      </c>
+      <c r="C50">
+        <v>8</v>
+      </c>
+      <c r="D50" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50" s="2">
+        <v>26124</v>
+      </c>
+      <c r="F50" s="2">
+        <v>0</v>
+      </c>
+      <c r="G50" s="2">
+        <v>5075.110384361461</v>
+      </c>
+      <c r="H50" s="2">
+        <v>1211.7352676</v>
+      </c>
+      <c r="I50" s="2">
+        <v>4156</v>
+      </c>
+      <c r="J50" s="3">
+        <v>1.9086926086800002</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>7500</v>
+      </c>
+      <c r="B51">
+        <v>75</v>
+      </c>
+      <c r="C51">
+        <v>8</v>
+      </c>
+      <c r="D51" t="s">
+        <v>2</v>
+      </c>
+      <c r="E51" s="2">
+        <v>20099</v>
+      </c>
+      <c r="F51" s="2">
+        <v>0</v>
+      </c>
+      <c r="G51" s="2">
+        <v>3904.6334257878193</v>
+      </c>
+      <c r="H51" s="2">
+        <v>3704.64</v>
+      </c>
+      <c r="I51" s="2">
+        <v>5988</v>
+      </c>
+      <c r="J51" s="3">
+        <v>6.3741599999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>7500</v>
+      </c>
+      <c r="B52">
+        <v>75</v>
+      </c>
+      <c r="C52">
+        <v>8</v>
+      </c>
+      <c r="D52" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="2">
+        <v>0</v>
+      </c>
+      <c r="F52" s="2">
+        <v>0</v>
+      </c>
+      <c r="G52" s="2">
+        <v>0</v>
+      </c>
+      <c r="H52" s="2">
+        <v>0</v>
+      </c>
+      <c r="I52" s="2">
+        <v>0</v>
+      </c>
+      <c r="J52" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>7500</v>
+      </c>
+      <c r="B53">
+        <v>75</v>
+      </c>
+      <c r="C53">
+        <v>9</v>
+      </c>
+      <c r="D53" t="s">
+        <v>5</v>
+      </c>
+      <c r="E53" s="2">
+        <v>27151</v>
+      </c>
+      <c r="F53" s="2">
+        <v>0</v>
+      </c>
+      <c r="G53" s="2">
+        <v>5274.6257099141794</v>
+      </c>
+      <c r="H53" s="2">
+        <v>1221.2138332</v>
+      </c>
+      <c r="I53" s="2">
+        <v>4156</v>
+      </c>
+      <c r="J53" s="3">
+        <v>1.92362298876</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>7500</v>
+      </c>
+      <c r="B54">
+        <v>75</v>
+      </c>
+      <c r="C54">
+        <v>9</v>
+      </c>
+      <c r="D54" t="s">
+        <v>2</v>
+      </c>
+      <c r="E54" s="2">
+        <v>20920</v>
+      </c>
+      <c r="F54" s="2">
+        <v>0</v>
+      </c>
+      <c r="G54" s="2">
+        <v>4064.1291242092234</v>
+      </c>
+      <c r="H54" s="2">
+        <v>3704.64</v>
+      </c>
+      <c r="I54" s="2">
+        <v>5988</v>
+      </c>
+      <c r="J54" s="3">
+        <v>6.3741599999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>7500</v>
+      </c>
+      <c r="B55">
+        <v>75</v>
+      </c>
+      <c r="C55">
+        <v>9</v>
+      </c>
+      <c r="D55" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="2">
+        <v>0</v>
+      </c>
+      <c r="F55" s="2">
+        <v>0</v>
+      </c>
+      <c r="G55" s="2">
+        <v>0</v>
+      </c>
+      <c r="H55" s="2">
+        <v>0</v>
+      </c>
+      <c r="I55" s="2">
+        <v>0</v>
+      </c>
+      <c r="J55" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>